<commit_message>
modified productslist excel file. added formatting. created new Base class to access newly created config.properties file.  Refactored package struture.  modified pom.xml to add build tag and allure reports dependencies.
</commit_message>
<xml_diff>
--- a/src/test/resources/datafiles/ProductsList.xlsx
+++ b/src/test/resources/datafiles/ProductsList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angha\eclipse-workspace\Avactis\src\test\resources\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080A5922-9FD0-4A03-9544-92669776B06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC7CAA6-91BC-43CD-8F75-7F66BEC0CEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="1790" windowWidth="19200" windowHeight="11170" xr2:uid="{BB58CDC0-0A2E-466D-BD3B-B7B322843004}"/>
+    <workbookView xWindow="6400" yWindow="1790" windowWidth="19200" windowHeight="11170" xr2:uid="{BB58CDC0-0A2E-466D-BD3B-B7B322843004}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="54">
   <si>
     <t xml:space="preserve">product_type_id   </t>
   </si>
@@ -264,7 +264,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -283,25 +283,11 @@
         <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -615,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5248925-0C5B-4238-8D4E-2089997E29A1}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1116,6 +1102,9 @@
       <c r="B25" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="C25" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D25" s="5" t="s">
         <v>30</v>
       </c>
@@ -1133,6 +1122,9 @@
       <c r="B26" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="C26" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>31</v>
       </c>
@@ -1150,6 +1142,9 @@
       <c r="B27" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="C27" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>32</v>
       </c>
@@ -1167,6 +1162,9 @@
       <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="C28" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>33</v>
       </c>
@@ -1184,6 +1182,9 @@
       <c r="B29" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="C29" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>34</v>
       </c>
@@ -1201,6 +1202,9 @@
       <c r="B30" s="5" t="s">
         <v>35</v>
       </c>
+      <c r="C30" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D30" s="5" t="s">
         <v>36</v>
       </c>
@@ -1218,6 +1222,9 @@
       <c r="B31" s="5" t="s">
         <v>35</v>
       </c>
+      <c r="C31" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D31" s="5" t="s">
         <v>37</v>
       </c>
@@ -1235,6 +1242,9 @@
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
+      <c r="C32" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D32" s="5" t="s">
         <v>38</v>
       </c>
@@ -1252,6 +1262,9 @@
       <c r="B33" s="5" t="s">
         <v>35</v>
       </c>
+      <c r="C33" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D33" s="5" t="s">
         <v>39</v>
       </c>
@@ -1264,7 +1277,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F33">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added log4j2, added checkout verification. order placed verification.
</commit_message>
<xml_diff>
--- a/src/test/resources/datafiles/ProductsList.xlsx
+++ b/src/test/resources/datafiles/ProductsList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angha\eclipse-workspace\Avactis\src\test\resources\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89CD513-6FD9-4DBB-B57B-D85CD6FF13E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26186A1-1E10-43AE-82B0-7FD7B3F29FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{10588F02-F978-4877-B51A-BD8431D1B5B6}"/>
+    <workbookView xWindow="640" yWindow="100" windowWidth="14660" windowHeight="11340" xr2:uid="{10588F02-F978-4877-B51A-BD8431D1B5B6}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCTS" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="51">
   <si>
     <t>product_id</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Digital Distribution</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -656,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B215B555-2954-4FF9-923F-9F7D69AE1DFD}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,7 +677,7 @@
     <col min="5" max="5" width="20.08984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -687,8 +693,14 @@
       <c r="E1" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3</v>
       </c>
@@ -704,8 +716,14 @@
       <c r="E2" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>6</v>
       </c>
@@ -721,8 +739,14 @@
       <c r="E3" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>8</v>
       </c>
@@ -738,8 +762,14 @@
       <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11</v>
       </c>
@@ -755,8 +785,14 @@
       <c r="E5" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15</v>
       </c>
@@ -772,8 +808,14 @@
       <c r="E6" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>18</v>
       </c>
@@ -789,8 +831,14 @@
       <c r="E7" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>28</v>
       </c>
@@ -806,8 +854,14 @@
       <c r="E8" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>499.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>31</v>
       </c>
@@ -823,8 +877,14 @@
       <c r="E9" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>799.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>32</v>
       </c>
@@ -840,8 +900,14 @@
       <c r="E10" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>33</v>
       </c>
@@ -857,8 +923,14 @@
       <c r="E11" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>34</v>
       </c>
@@ -874,8 +946,14 @@
       <c r="E12" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>35</v>
       </c>
@@ -891,8 +969,14 @@
       <c r="E13" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>25.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>36</v>
       </c>
@@ -908,8 +992,14 @@
       <c r="E14" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>47</v>
       </c>
@@ -925,8 +1015,14 @@
       <c r="E15" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>37</v>
       </c>
@@ -942,8 +1038,14 @@
       <c r="E16" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>89</v>
       </c>
@@ -959,8 +1061,14 @@
       <c r="E17" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>90</v>
       </c>
@@ -976,8 +1084,14 @@
       <c r="E18" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>91</v>
       </c>
@@ -993,8 +1107,14 @@
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>97</v>
       </c>
@@ -1010,8 +1130,14 @@
       <c r="E20" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>33.450000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>106</v>
       </c>
@@ -1027,8 +1153,14 @@
       <c r="E21" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>108</v>
       </c>
@@ -1044,8 +1176,14 @@
       <c r="E22" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>48.59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>116</v>
       </c>
@@ -1061,8 +1199,14 @@
       <c r="E23" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>125</v>
       </c>
@@ -1078,8 +1222,14 @@
       <c r="E24" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>126</v>
       </c>
@@ -1095,8 +1245,14 @@
       <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>130</v>
       </c>
@@ -1112,8 +1268,14 @@
       <c r="E26" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>229.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>133</v>
       </c>
@@ -1129,8 +1291,14 @@
       <c r="E27" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>49.95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>138</v>
       </c>
@@ -1146,8 +1314,14 @@
       <c r="E28" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>139</v>
       </c>
@@ -1163,8 +1337,14 @@
       <c r="E29" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>161</v>
       </c>
@@ -1180,8 +1360,14 @@
       <c r="E30" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>169</v>
       </c>
@@ -1196,6 +1382,12 @@
       </c>
       <c r="E31" s="4" t="s">
         <v>44</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>9.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>